<commit_message>
Changes to data - now reflected in essay descs
</commit_message>
<xml_diff>
--- a/data/Essay_Set_Descriptions/essay_set_descriptions.xlsx
+++ b/data/Essay_Set_Descriptions/essay_set_descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>essay_set</t>
   </si>
@@ -31,6 +31,9 @@
     <t>training_set_size</t>
   </si>
   <si>
+    <t>test_set_size</t>
+  </si>
+  <si>
     <t>has_domain1rater1</t>
   </si>
   <si>
@@ -65,6 +68,9 @@
   </si>
   <si>
     <t>source dependent responses</t>
+  </si>
+  <si>
+    <t>valid_set_size</t>
   </si>
 </sst>
 </file>
@@ -403,18 +409,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="5" max="6" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,40 +435,46 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
-        <v>11</v>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,22 +485,22 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="E2">
+        <v>589</v>
+      </c>
+      <c r="F2">
+        <v>594</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>12</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -496,13 +509,19 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -516,31 +535,31 @@
         <v>1800</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="F3">
+        <v>600</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>4</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -548,13 +567,19 @@
       <c r="O3">
         <v>1</v>
       </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -563,19 +588,19 @@
         <v>1726</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>568</v>
       </c>
       <c r="F4">
+        <v>564</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -584,18 +609,24 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -604,19 +635,19 @@
         <v>1772</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>586</v>
       </c>
       <c r="F5">
+        <v>590</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -625,18 +656,24 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -645,19 +682,19 @@
         <v>1805</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>601</v>
       </c>
       <c r="F6">
+        <v>600</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -666,18 +703,24 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -686,19 +729,19 @@
         <v>1800</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F7">
+        <v>600</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -707,9 +750,109 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>1569</v>
+      </c>
+      <c r="E8">
+        <v>441</v>
+      </c>
+      <c r="F8">
+        <v>454</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>723</v>
+      </c>
+      <c r="E9">
+        <v>233</v>
+      </c>
+      <c r="F9">
+        <v>252</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>0</v>
       </c>
     </row>

</xml_diff>